<commit_message>
solo los primeros campos
</commit_message>
<xml_diff>
--- a/html_to_excel/output_problemas.xlsx
+++ b/html_to_excel/output_problemas.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Auditoría Problemas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,65 +436,55 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>Remediation</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>PowerShell Script</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Remediation</t>
+          <t>Returned Value</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>PowerShell Script</t>
+          <t>Default Value</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Returned Value</t>
+          <t>Expected Value</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Default Value</t>
+          <t>Impact</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Expected Value</t>
+          <t>Likelihood</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Impact</t>
+          <t>Priority</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Likelihood</t>
+          <t>RiskRating</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>RiskRating</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>References</t>
         </is>
@@ -503,21 +493,59 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CIS MOff 1.1.2 - Less than 2 emergency access accounts have been defined</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+          <t>Enabling the default Teams DLP policy rule in Microsoft 365 helps protect an organization's sensitive information by preventing accidental sharing or leakage of that information in Teams conversations and channels.</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Use the PowerShell script to create a new DLPCompliancePolicy or review the policies existence and if they are enabled.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>New-DlpCompliancePolicy -Name "SSN Teams Policy" -Comment "SSN Teams Policy" -TeamsLocation All -Mode Enable</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Default Value:Enable</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Enable</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Enable</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Informational</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Learn about data loss prevention</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>